<commit_message>
corrected match 13 start time
</commit_message>
<xml_diff>
--- a/tournaments/2025-mens-club-world-cup.xlsx
+++ b/tournaments/2025-mens-club-world-cup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/tournaments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFABB130-D7C2-2D41-A04C-68F3FD6DDDC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C29078-70EE-264C-AF30-CB3C36AB52DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="940" windowWidth="33880" windowHeight="14380" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
+    <workbookView xWindow="160" yWindow="940" windowWidth="33880" windowHeight="14380" activeTab="1" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tournament" sheetId="8" r:id="rId1"/>
@@ -1872,7 +1872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393FFACE-29F0-47F7-B7AD-389E0D6667C5}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2356,8 +2356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ABE575-0207-4299-82CD-74F27B6194DA}">
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E64"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2646,7 +2646,7 @@
         <v>21</v>
       </c>
       <c r="D13" s="1">
-        <v>45825.791666666664</v>
+        <v>45826.041666666664</v>
       </c>
       <c r="E13">
         <v>4</v>

</xml_diff>

<commit_message>
D4 team is now LAFC (not lyon)
</commit_message>
<xml_diff>
--- a/tournaments/2025-mens-club-world-cup.xlsx
+++ b/tournaments/2025-mens-club-world-cup.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/tournaments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C29078-70EE-264C-AF30-CB3C36AB52DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8462A593-DD7F-5445-887B-DBD69F322153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="940" windowWidth="33880" windowHeight="14380" activeTab="1" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
   </bookViews>
@@ -541,9 +541,6 @@
     <t>CHE</t>
   </si>
   <si>
-    <t>LEO</t>
-  </si>
-  <si>
     <t>RIV</t>
   </si>
   <si>
@@ -1280,6 +1277,9 @@
   </si>
   <si>
     <t>America/New_York</t>
+  </si>
+  <si>
+    <t>LAF</t>
   </si>
 </sst>
 </file>
@@ -1876,7 +1876,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="A5:XFD5"/>
+      <selection pane="bottomRight" sqref="A1:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1955,28 +1955,28 @@
         <v>91</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -2010,10 +2010,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>410</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>411</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>412</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -2086,22 +2086,22 @@
         <v>78</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>130</v>
@@ -2115,28 +2115,28 @@
         <v>79</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>393</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -2202,28 +2202,28 @@
         <v>82</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -2231,28 +2231,28 @@
         <v>83</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -2357,7 +2357,7 @@
   <dimension ref="A1:K64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3741,8 +3741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7827E4A0-E10B-4512-807E-A38B484A1AB9}">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3880,7 +3880,7 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>166</v>
+        <v>412</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -3888,7 +3888,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -3896,7 +3896,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -3904,7 +3904,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -3912,7 +3912,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -3920,7 +3920,7 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -3928,7 +3928,7 @@
         <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -3936,7 +3936,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -3944,7 +3944,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -3952,7 +3952,7 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -3960,7 +3960,7 @@
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -3968,7 +3968,7 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -3976,7 +3976,7 @@
         <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -3984,7 +3984,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -3992,7 +3992,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -4000,7 +4000,7 @@
         <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -4008,7 +4008,7 @@
         <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -4070,10 +4070,10 @@
         <v>102</v>
       </c>
       <c r="B2" t="s">
+        <v>394</v>
+      </c>
+      <c r="J2" t="s">
         <v>395</v>
-      </c>
-      <c r="J2" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -4081,10 +4081,10 @@
         <v>103</v>
       </c>
       <c r="B3" t="s">
+        <v>396</v>
+      </c>
+      <c r="J3" t="s">
         <v>397</v>
-      </c>
-      <c r="J3" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -4092,10 +4092,10 @@
         <v>105</v>
       </c>
       <c r="B4" t="s">
+        <v>398</v>
+      </c>
+      <c r="J4" t="s">
         <v>399</v>
-      </c>
-      <c r="J4" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -4103,10 +4103,10 @@
         <v>100</v>
       </c>
       <c r="B5" t="s">
+        <v>400</v>
+      </c>
+      <c r="J5" t="s">
         <v>401</v>
-      </c>
-      <c r="J5" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -4114,10 +4114,10 @@
         <v>106</v>
       </c>
       <c r="B6" t="s">
+        <v>402</v>
+      </c>
+      <c r="J6" t="s">
         <v>403</v>
-      </c>
-      <c r="J6" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -4125,10 +4125,10 @@
         <v>107</v>
       </c>
       <c r="B7" t="s">
+        <v>408</v>
+      </c>
+      <c r="J7" t="s">
         <v>409</v>
-      </c>
-      <c r="J7" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -4136,10 +4136,10 @@
         <v>101</v>
       </c>
       <c r="B8" t="s">
+        <v>404</v>
+      </c>
+      <c r="J8" t="s">
         <v>405</v>
-      </c>
-      <c r="J8" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -4147,10 +4147,10 @@
         <v>104</v>
       </c>
       <c r="B9" t="s">
+        <v>406</v>
+      </c>
+      <c r="J9" t="s">
         <v>407</v>
-      </c>
-      <c r="J9" t="s">
-        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -4213,930 +4213,930 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>291</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>298</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>304</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>312</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>228</v>
-      </c>
       <c r="C12" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G12" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>315</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>230</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H13" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>317</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>321</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>324</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="H17" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>389</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>241</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="I18" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="H20" s="2" t="s">
+      <c r="I20" s="2" t="s">
         <v>331</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>338</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="H22" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="H23" s="2" t="s">
+      <c r="I23" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="H24" s="2" t="s">
+      <c r="I24" s="2" t="s">
         <v>341</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="H25" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="H25" s="2" t="s">
-        <v>349</v>
-      </c>
       <c r="I25" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="G26" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="I26" s="2" t="s">
         <v>264</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="H27" s="2" t="s">
+      <c r="I27" s="2" t="s">
         <v>351</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="H28" s="2" t="s">
+      <c r="I28" s="2" t="s">
         <v>356</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="F29" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="H29" s="2" t="s">
+      <c r="I29" s="2" t="s">
         <v>360</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="G30" s="2" t="s">
+      <c r="H30" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="I30" s="2" t="s">
         <v>366</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="H31" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="H32" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="G33" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="G33" s="2" t="s">
+      <c r="H33" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="I33" s="2" t="s">
         <v>377</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -5165,16 +5165,16 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B1" t="s">
         <v>62</v>
       </c>
       <c r="C1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" t="s">
         <v>192</v>
-      </c>
-      <c r="D1" t="s">
-        <v>193</v>
       </c>
       <c r="E1" t="s">
         <v>63</v>
@@ -5183,13 +5183,13 @@
         <v>66</v>
       </c>
       <c r="G1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="J1" t="s">
         <v>93</v>
@@ -5209,10 +5209,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E2" s="6">
         <v>0.83333333333333337</v>
@@ -5253,16 +5253,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E3" s="6">
         <v>0.5</v>
       </c>
       <c r="F3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G3" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -5297,16 +5297,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E4" s="6">
         <v>0.625</v>
       </c>
       <c r="F4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G4" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -5341,16 +5341,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E5" s="6">
         <v>0.75</v>
       </c>
       <c r="F5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G5" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -5385,10 +5385,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E6" s="6">
         <v>0.91666666666666663</v>
@@ -5429,10 +5429,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D7" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E7" s="6">
         <v>0.625</v>
@@ -5456,9 +5456,9 @@
         <f>INDEX(seeds[seed],MATCH(UPPER(Table6[[#This Row],[home-club]]),seeds[team],0))</f>
         <v>D3</v>
       </c>
-      <c r="K7" t="str">
+      <c r="K7" t="e">
         <f>INDEX(seeds[seed],MATCH(UPPER(Table6[[#This Row],[away-club]]),seeds[team],0))</f>
-        <v>D4</v>
+        <v>#N/A</v>
       </c>
       <c r="L7">
         <f>_xlfn.NUMBERVALUE(_xlfn.TEXTAFTER(INDEX(tournament[key],MATCH(Table6[[#This Row],[location]],tournament[en],0)),"."))</f>
@@ -5473,10 +5473,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E8" s="6">
         <v>0.75</v>
@@ -5517,10 +5517,10 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E9" s="6">
         <v>0.875</v>
@@ -5561,16 +5561,16 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E10" s="6">
         <v>0.5</v>
       </c>
       <c r="F10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G10" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -5605,10 +5605,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E11" s="6">
         <v>0.625</v>
@@ -5649,16 +5649,16 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D12" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E12" s="6">
         <v>0.75</v>
       </c>
       <c r="F12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G12" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -5693,16 +5693,16 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D13" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E13" s="6">
         <v>0.625</v>
       </c>
       <c r="F13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G13" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -5737,10 +5737,10 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D14" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E14" s="6">
         <v>0.5</v>
@@ -5781,10 +5781,10 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D15" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E15" s="6">
         <v>0.625</v>
@@ -5825,16 +5825,16 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D16" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E16" s="6">
         <v>0.75</v>
       </c>
       <c r="F16" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G16" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -5869,10 +5869,10 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D17" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E17" s="6">
         <v>0.875</v>
@@ -5913,16 +5913,16 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E18" s="6">
         <v>0.5</v>
       </c>
       <c r="F18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G18" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -5957,10 +5957,10 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D19" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E19" s="6">
         <v>0.625</v>
@@ -6001,10 +6001,10 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E20" s="6">
         <v>0.75</v>
@@ -6045,16 +6045,16 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E21" s="6">
         <v>0.875</v>
       </c>
       <c r="F21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G21" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -6089,16 +6089,16 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D22" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E22" s="6">
         <v>0.5</v>
       </c>
       <c r="F22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G22" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -6133,10 +6133,10 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D23" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E23" s="6">
         <v>0.58333333333333337</v>
@@ -6177,10 +6177,10 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E24" s="6">
         <v>0.75</v>
@@ -6200,9 +6200,9 @@
         <f>INDEX(club[key],MATCH(Table6[[#This Row],[away]],club[en],0))</f>
         <v>est</v>
       </c>
-      <c r="J24" t="str">
+      <c r="J24" t="e">
         <f>INDEX(seeds[seed],MATCH(UPPER(Table6[[#This Row],[home-club]]),seeds[team],0))</f>
-        <v>D4</v>
+        <v>#N/A</v>
       </c>
       <c r="K24" t="str">
         <f>INDEX(seeds[seed],MATCH(UPPER(Table6[[#This Row],[away-club]]),seeds[team],0))</f>
@@ -6221,10 +6221,10 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E25" s="6">
         <v>0.875</v>
@@ -6265,16 +6265,16 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D26" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E26" s="6">
         <v>0.5</v>
       </c>
       <c r="F26" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G26" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -6309,10 +6309,10 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D27" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E27" s="6">
         <v>0.625</v>
@@ -6353,16 +6353,16 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E28" s="6">
         <v>0.75</v>
       </c>
       <c r="F28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G28" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -6397,16 +6397,16 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D29" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E29" s="6">
         <v>0.875</v>
       </c>
       <c r="F29" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G29" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -6441,10 +6441,10 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D30" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E30" s="6">
         <v>0.5</v>
@@ -6485,10 +6485,10 @@
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D31" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E31" s="6">
         <v>0.625</v>
@@ -6529,10 +6529,10 @@
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D32" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E32" s="6">
         <v>0.75</v>
@@ -6573,10 +6573,10 @@
         <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D33" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E33" s="6">
         <v>0.875</v>
@@ -6617,10 +6617,10 @@
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D34" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E34" s="6">
         <v>0.625</v>
@@ -6661,16 +6661,16 @@
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D35" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E35" s="6">
         <v>0.625</v>
       </c>
       <c r="F35" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G35" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -6705,10 +6705,10 @@
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D36" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E36" s="6">
         <v>0.875</v>
@@ -6749,16 +6749,16 @@
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D37" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E37" s="6">
         <v>0.875</v>
       </c>
       <c r="F37" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G37" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -6793,10 +6793,10 @@
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D38" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E38" s="6">
         <v>0.625</v>
@@ -6837,10 +6837,10 @@
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D39" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E39" s="6">
         <v>0.625</v>
@@ -6881,16 +6881,16 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D40" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E40" s="6">
         <v>0.875</v>
       </c>
       <c r="F40" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G40" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -6904,9 +6904,9 @@
         <f>INDEX(club[key],MATCH(Table6[[#This Row],[away]],club[en],0))</f>
         <v>fla</v>
       </c>
-      <c r="J40" t="str">
+      <c r="J40" t="e">
         <f>INDEX(seeds[seed],MATCH(UPPER(Table6[[#This Row],[home-club]]),seeds[team],0))</f>
-        <v>D4</v>
+        <v>#N/A</v>
       </c>
       <c r="K40" t="str">
         <f>INDEX(seeds[seed],MATCH(UPPER(Table6[[#This Row],[away-club]]),seeds[team],0))</f>
@@ -6925,10 +6925,10 @@
         <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D41" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E41" s="6">
         <v>0.875</v>
@@ -6969,16 +6969,16 @@
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D42" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E42" s="6">
         <v>0.625</v>
       </c>
       <c r="F42" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G42" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -7013,10 +7013,10 @@
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D43" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E43" s="6">
         <v>0.625</v>
@@ -7057,10 +7057,10 @@
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D44" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E44" s="6">
         <v>0.875</v>
@@ -7101,16 +7101,16 @@
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D45" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E45" s="6">
         <v>0.875</v>
       </c>
       <c r="F45" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G45" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -7145,16 +7145,16 @@
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D46" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E46" s="6">
         <v>0.625</v>
       </c>
       <c r="F46" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G46" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -7189,10 +7189,10 @@
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D47" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E47" s="6">
         <v>0.625</v>
@@ -7233,10 +7233,10 @@
         <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D48" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E48" s="6">
         <v>0.875</v>
@@ -7277,10 +7277,10 @@
         <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D49" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E49" s="6">
         <v>0.875</v>
@@ -7550,7 +7550,7 @@
         <v>0.875</v>
       </c>
       <c r="F55" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G55" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -7682,7 +7682,7 @@
         <v>0.625</v>
       </c>
       <c r="F58" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G58" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -7814,7 +7814,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="F61" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G61" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -7858,7 +7858,7 @@
         <v>0.625</v>
       </c>
       <c r="F62" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G62" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -7902,7 +7902,7 @@
         <v>0.625</v>
       </c>
       <c r="F63" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G63" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>
@@ -7946,7 +7946,7 @@
         <v>0.625</v>
       </c>
       <c r="F64" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G64" s="7">
         <f>Table6[[#This Row],[date]]+Table6[[#This Row],[time]]+(4/24)</f>

</xml_diff>